<commit_message>
Correcting coal (ton) formatting
</commit_message>
<xml_diff>
--- a/src/data-graphql/production_volumes.xlsx
+++ b/src/data-graphql/production_volumes.xlsx
@@ -98,7 +98,7 @@
     <t>Native American</t>
   </si>
   <si>
-    <t>Coal (ton)</t>
+    <t>Coal Prod Vol (ton)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:F1057"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1036" workbookViewId="0">
-      <selection activeCell="E1057" sqref="E1057"/>
+      <selection activeCell="S1055" sqref="S1055"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
format update on production file
</commit_message>
<xml_diff>
--- a/src/data-graphql/production_volumes.xlsx
+++ b/src/data-graphql/production_volumes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isemibnas01\onrr\SHARE\NRRD\Data\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mentastc\Documents\GitHub\doi-extractives-data\src\data-graphql\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A1047" workbookViewId="0">
+      <selection activeCell="H1078" sqref="H1078"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21980,13 +21980,13 @@
       <c r="C1072" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1072" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1072" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1072" s="8">
+      <c r="D1072" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1072" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1072" s="9">
         <v>25622939.410871997</v>
       </c>
     </row>
@@ -22000,13 +22000,13 @@
       <c r="C1073" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1073" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1073" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1073" s="8">
+      <c r="D1073" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1073" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1073" s="9">
         <v>5947699.9094679998</v>
       </c>
     </row>
@@ -22020,13 +22020,13 @@
       <c r="C1074" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1074" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1074" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1074" s="8">
+      <c r="D1074" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1074" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1074" s="9">
         <v>94243257.760961995</v>
       </c>
     </row>
@@ -22040,13 +22040,13 @@
       <c r="C1075" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1075" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1075" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1075" s="8">
+      <c r="D1075" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1075" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1075" s="9">
         <v>59154063.83901</v>
       </c>
     </row>
@@ -22057,7 +22057,7 @@
       <c r="B1076" s="6">
         <v>2019</v>
       </c>
-      <c r="C1076" s="4" t="s">
+      <c r="C1076" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D1076" s="4" t="s">
@@ -22080,13 +22080,13 @@
       <c r="C1077" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1077" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1077" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1077" s="8">
+      <c r="D1077" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1077" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1077" s="9">
         <v>271559636.02770197</v>
       </c>
     </row>
@@ -22100,13 +22100,13 @@
       <c r="C1078" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1078" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1078" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1078" s="8">
+      <c r="D1078" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1078" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1078" s="9">
         <v>21951668.853908997</v>
       </c>
     </row>
@@ -22140,13 +22140,13 @@
       <c r="C1080" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1080" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1080" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1080" s="8">
+      <c r="D1080" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1080" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1080" s="9">
         <v>29063441.331801005</v>
       </c>
     </row>
@@ -22160,13 +22160,13 @@
       <c r="C1081" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1081" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1081" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1081" s="8">
+      <c r="D1081" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1081" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1081" s="9">
         <v>6720610.6272520004</v>
       </c>
     </row>

</xml_diff>